<commit_message>
finished 10 novice users data
</commit_message>
<xml_diff>
--- a/data/userdata-micropipette-10-16-15.xlsx
+++ b/data/userdata-micropipette-10-16-15.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fahad\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fahad\Documents\Git Bash\micropipette\micropipette\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22455" windowHeight="8610" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22455" windowHeight="8610"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,10 @@
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
     <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet10" sheetId="12" r:id="rId10"/>
+    <sheet name="Expert 1" sheetId="10" r:id="rId11"/>
+    <sheet name="Expert 2" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="3">
   <si>
     <t>Trial</t>
   </si>
@@ -359,7 +363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -446,6 +450,161 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>10</v>
+      </c>
+      <c r="D1">
+        <v>20</v>
+      </c>
+      <c r="E1">
+        <v>50</v>
+      </c>
+      <c r="F1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D3">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="E3">
+        <v>54.1</v>
+      </c>
+      <c r="F3">
+        <v>193.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>10.9</v>
+      </c>
+      <c r="D4">
+        <v>16.5</v>
+      </c>
+      <c r="E4">
+        <v>41.1</v>
+      </c>
+      <c r="F4">
+        <v>197.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>11.8</v>
+      </c>
+      <c r="D5">
+        <v>16.3</v>
+      </c>
+      <c r="E5">
+        <v>42</v>
+      </c>
+      <c r="F5">
+        <v>197.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>10</v>
+      </c>
+      <c r="D1">
+        <v>20</v>
+      </c>
+      <c r="E1">
+        <v>50</v>
+      </c>
+      <c r="F1">
+        <v>200</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -909,7 +1068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1001,7 +1160,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J7"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,15 +1194,142 @@
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="C3">
+        <v>7.6</v>
+      </c>
+      <c r="D3">
+        <v>25.9</v>
+      </c>
+      <c r="E3">
+        <v>41.7</v>
+      </c>
+      <c r="F3">
+        <v>190.8</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
+      </c>
+      <c r="C4">
+        <v>9.6</v>
+      </c>
+      <c r="D4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="E4">
+        <v>48.4</v>
+      </c>
+      <c r="F4">
+        <v>199.4</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>20.3</v>
+      </c>
+      <c r="E5">
+        <v>48.7</v>
+      </c>
+      <c r="F5">
+        <v>202.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>10</v>
+      </c>
+      <c r="D1">
+        <v>20</v>
+      </c>
+      <c r="E1">
+        <v>50</v>
+      </c>
+      <c r="F1">
+        <v>200</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>10.9</v>
+      </c>
+      <c r="D3">
+        <v>15.9</v>
+      </c>
+      <c r="E3">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="F3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="E4">
+        <v>47.1</v>
+      </c>
+      <c r="F4">
+        <v>182.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>11.1</v>
+      </c>
+      <c r="D5">
+        <v>19.2</v>
+      </c>
+      <c r="E5">
+        <v>47.1</v>
+      </c>
+      <c r="F5">
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
put together all data
</commit_message>
<xml_diff>
--- a/data/userdata-micropipette-10-16-15.xlsx
+++ b/data/userdata-micropipette-10-16-15.xlsx
@@ -12,18 +12,19 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22455" windowHeight="8610"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
-    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
-    <sheet name="Sheet10" sheetId="12" r:id="rId10"/>
-    <sheet name="Expert 1" sheetId="10" r:id="rId11"/>
-    <sheet name="Expert 2" sheetId="13" r:id="rId12"/>
+    <sheet name="All Data" sheetId="14" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId7"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId8"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId9"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId10"/>
+    <sheet name="Sheet10" sheetId="12" r:id="rId11"/>
+    <sheet name="Expert 1" sheetId="10" r:id="rId12"/>
+    <sheet name="Expert 2" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="10">
   <si>
     <t>Trial</t>
   </si>
@@ -45,11 +46,35 @@
   <si>
     <t>weight in mg</t>
   </si>
+  <si>
+    <t>Systematic Error</t>
+  </si>
+  <si>
+    <t>Random Error</t>
+  </si>
+  <si>
+    <t>Average in µG</t>
+  </si>
+  <si>
+    <t>10µL</t>
+  </si>
+  <si>
+    <t>20µL</t>
+  </si>
+  <si>
+    <t>50µL</t>
+  </si>
+  <si>
+    <t>200µL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.00\ "/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -79,8 +104,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -361,17 +388,616 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
   </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>8.1</v>
+      </c>
+      <c r="D3">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="E3">
+        <v>48.5</v>
+      </c>
+      <c r="F3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>10.4</v>
+      </c>
+      <c r="D4">
+        <v>20.6</v>
+      </c>
+      <c r="E4">
+        <v>45.8</v>
+      </c>
+      <c r="F4">
+        <v>185.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>10.6</v>
+      </c>
+      <c r="D5">
+        <v>18.7</v>
+      </c>
+      <c r="E5">
+        <v>41.6</v>
+      </c>
+      <c r="F5">
+        <v>186.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>3.8</v>
+      </c>
+      <c r="D6">
+        <v>22.4</v>
+      </c>
+      <c r="E6">
+        <v>48.3</v>
+      </c>
+      <c r="F6">
+        <v>176.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>7.4</v>
+      </c>
+      <c r="D7">
+        <v>16.2</v>
+      </c>
+      <c r="E7">
+        <v>49</v>
+      </c>
+      <c r="F7">
+        <v>182.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D8">
+        <v>22.3</v>
+      </c>
+      <c r="E8">
+        <v>48.8</v>
+      </c>
+      <c r="F8">
+        <v>193.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>6.4</v>
+      </c>
+      <c r="D9">
+        <v>17.8</v>
+      </c>
+      <c r="E9">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="F9">
+        <v>183.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>6.5</v>
+      </c>
+      <c r="D10">
+        <v>16.3</v>
+      </c>
+      <c r="E10">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="F10">
+        <v>183.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>7.8</v>
+      </c>
+      <c r="D11">
+        <v>13.5</v>
+      </c>
+      <c r="E11">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="F11">
+        <v>187.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>7.3</v>
+      </c>
+      <c r="D12">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="E12">
+        <v>44.7</v>
+      </c>
+      <c r="F12">
+        <v>175.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>9.4</v>
+      </c>
+      <c r="D13">
+        <v>20.7</v>
+      </c>
+      <c r="E13">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="F13">
+        <v>203.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>9.6</v>
+      </c>
+      <c r="D14">
+        <v>17.2</v>
+      </c>
+      <c r="E14">
+        <v>44.6</v>
+      </c>
+      <c r="F14">
+        <v>193.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>14.5</v>
+      </c>
+      <c r="D15">
+        <v>20.5</v>
+      </c>
+      <c r="E15">
+        <v>44.4</v>
+      </c>
+      <c r="F15">
+        <v>186.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>4.2</v>
+      </c>
+      <c r="D16">
+        <v>19.7</v>
+      </c>
+      <c r="E16">
+        <v>49.4</v>
+      </c>
+      <c r="F16">
+        <v>185.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>6.6</v>
+      </c>
+      <c r="D17">
+        <v>20.9</v>
+      </c>
+      <c r="E17">
+        <v>50.5</v>
+      </c>
+      <c r="F17">
+        <v>189.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>3.3</v>
+      </c>
+      <c r="D18">
+        <v>15.5</v>
+      </c>
+      <c r="E18">
+        <v>48.2</v>
+      </c>
+      <c r="F18">
+        <v>187.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D19">
+        <v>11.2</v>
+      </c>
+      <c r="E19">
+        <v>44.8</v>
+      </c>
+      <c r="F19">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>12.9</v>
+      </c>
+      <c r="D20">
+        <v>23.4</v>
+      </c>
+      <c r="E20">
+        <v>67</v>
+      </c>
+      <c r="F20">
+        <v>192.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>5.5</v>
+      </c>
+      <c r="D21">
+        <v>16.2</v>
+      </c>
+      <c r="E21">
+        <v>43.6</v>
+      </c>
+      <c r="F21">
+        <v>185.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>9.1</v>
+      </c>
+      <c r="D22">
+        <v>16.2</v>
+      </c>
+      <c r="E22">
+        <v>43.3</v>
+      </c>
+      <c r="F22">
+        <v>185.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>9.9</v>
+      </c>
+      <c r="D23">
+        <v>16.5</v>
+      </c>
+      <c r="E23">
+        <v>44.1</v>
+      </c>
+      <c r="F23">
+        <v>187.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>7.6</v>
+      </c>
+      <c r="D24">
+        <v>25.9</v>
+      </c>
+      <c r="E24">
+        <v>41.7</v>
+      </c>
+      <c r="F24">
+        <v>190.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>9.6</v>
+      </c>
+      <c r="D25">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="E25">
+        <v>48.4</v>
+      </c>
+      <c r="F25">
+        <v>199.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>20.3</v>
+      </c>
+      <c r="E26">
+        <v>48.7</v>
+      </c>
+      <c r="F26">
+        <v>202.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>10.9</v>
+      </c>
+      <c r="D27">
+        <v>15.9</v>
+      </c>
+      <c r="E27">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="F27">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D28">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="E28">
+        <v>47.1</v>
+      </c>
+      <c r="F28">
+        <v>182.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>11.1</v>
+      </c>
+      <c r="D29">
+        <v>19.2</v>
+      </c>
+      <c r="E29">
+        <v>47.1</v>
+      </c>
+      <c r="F29">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D30">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="E30">
+        <v>54.1</v>
+      </c>
+      <c r="F30">
+        <v>193.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>10.9</v>
+      </c>
+      <c r="D31">
+        <v>16.5</v>
+      </c>
+      <c r="E31">
+        <v>41.1</v>
+      </c>
+      <c r="F31">
+        <v>197.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>11.8</v>
+      </c>
+      <c r="D32">
+        <v>16.3</v>
+      </c>
+      <c r="E32">
+        <v>42</v>
+      </c>
+      <c r="F32">
+        <v>197.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="2">
+        <f>AVERAGE(C3:C32)</f>
+        <v>8.5933333333333337</v>
+      </c>
+      <c r="D34" s="2">
+        <f>AVERAGE(D3:D32)</f>
+        <v>18.243333333333329</v>
+      </c>
+      <c r="E34" s="2">
+        <f>AVERAGE(E3:E32)</f>
+        <v>45.676666666666655</v>
+      </c>
+      <c r="F34" s="2">
+        <f>AVERAGE(F3:F32)</f>
+        <v>188.83666666666667</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="1">
+        <f>((C34-10)/10)</f>
+        <v>-0.14066666666666663</v>
+      </c>
+      <c r="D36" s="1">
+        <f>(D34-20)/20</f>
+        <v>-8.7833333333333569E-2</v>
+      </c>
+      <c r="E36" s="1">
+        <f>(E34-50)/50</f>
+        <v>-8.64666666666669E-2</v>
+      </c>
+      <c r="F36" s="1">
+        <f>(F34-200)/200</f>
+        <v>-5.5816666666666633E-2</v>
+      </c>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="2" t="e">
+        <f ca="1">(least((C3:C32),1)-C34)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="A3:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -403,16 +1029,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>8.1</v>
+        <v>10.9</v>
       </c>
       <c r="D3">
-        <v>16.399999999999999</v>
+        <v>15.9</v>
       </c>
       <c r="E3">
-        <v>48.5</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="F3">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -420,16 +1046,16 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>10.4</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="D4">
-        <v>20.6</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="E4">
-        <v>45.8</v>
+        <v>47.1</v>
       </c>
       <c r="F4">
-        <v>185.7</v>
+        <v>182.6</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -437,16 +1063,16 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>10.6</v>
+        <v>11.1</v>
       </c>
       <c r="D5">
-        <v>18.7</v>
+        <v>19.2</v>
       </c>
       <c r="E5">
-        <v>41.6</v>
+        <v>47.1</v>
       </c>
       <c r="F5">
-        <v>186.4</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -454,12 +1080,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F5" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,7 +1168,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -597,7 +1223,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -614,10 +1240,14 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F5" sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -649,16 +1279,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>3.8</v>
+        <v>8.1</v>
       </c>
       <c r="D3">
-        <v>22.4</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="E3">
-        <v>48.3</v>
+        <v>48.5</v>
       </c>
       <c r="F3">
-        <v>176.5</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -666,16 +1296,16 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>7.4</v>
+        <v>10.4</v>
       </c>
       <c r="D4">
-        <v>16.2</v>
+        <v>20.6</v>
       </c>
       <c r="E4">
-        <v>49</v>
+        <v>45.8</v>
       </c>
       <c r="F4">
-        <v>182.6</v>
+        <v>185.7</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -683,16 +1313,16 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>9.1999999999999993</v>
+        <v>10.6</v>
       </c>
       <c r="D5">
-        <v>22.3</v>
+        <v>18.7</v>
       </c>
       <c r="E5">
-        <v>48.8</v>
+        <v>41.6</v>
       </c>
       <c r="F5">
-        <v>193.7</v>
+        <v>186.4</v>
       </c>
     </row>
   </sheetData>
@@ -705,7 +1335,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F5" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,16 +1370,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>6.4</v>
+        <v>3.8</v>
       </c>
       <c r="D3">
-        <v>17.8</v>
+        <v>22.4</v>
       </c>
       <c r="E3">
-        <v>38.799999999999997</v>
+        <v>48.3</v>
       </c>
       <c r="F3">
-        <v>183.9</v>
+        <v>176.5</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -757,16 +1387,16 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>6.5</v>
+        <v>7.4</v>
       </c>
       <c r="D4">
-        <v>16.3</v>
+        <v>16.2</v>
       </c>
       <c r="E4">
-        <v>38.299999999999997</v>
+        <v>49</v>
       </c>
       <c r="F4">
-        <v>183.1</v>
+        <v>182.6</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -774,16 +1404,16 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>7.8</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="D5">
-        <v>13.5</v>
+        <v>22.3</v>
       </c>
       <c r="E5">
-        <v>37.799999999999997</v>
+        <v>48.8</v>
       </c>
       <c r="F5">
-        <v>187.5</v>
+        <v>193.7</v>
       </c>
     </row>
   </sheetData>
@@ -796,7 +1426,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F5" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,16 +1461,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>7.3</v>
+        <v>6.4</v>
       </c>
       <c r="D3">
-        <v>9.8000000000000007</v>
+        <v>17.8</v>
       </c>
       <c r="E3">
-        <v>44.7</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="F3">
-        <v>175.8</v>
+        <v>183.9</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -848,16 +1478,16 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>9.4</v>
+        <v>6.5</v>
       </c>
       <c r="D4">
-        <v>20.7</v>
+        <v>16.3</v>
       </c>
       <c r="E4">
         <v>38.299999999999997</v>
       </c>
       <c r="F4">
-        <v>203.1</v>
+        <v>183.1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -865,16 +1495,16 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>9.6</v>
+        <v>7.8</v>
       </c>
       <c r="D5">
-        <v>17.2</v>
+        <v>13.5</v>
       </c>
       <c r="E5">
-        <v>44.6</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="F5">
-        <v>193.4</v>
+        <v>187.5</v>
       </c>
     </row>
   </sheetData>
@@ -887,7 +1517,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F5" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,16 +1552,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>14.5</v>
+        <v>7.3</v>
       </c>
       <c r="D3">
-        <v>20.5</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="E3">
-        <v>44.4</v>
+        <v>44.7</v>
       </c>
       <c r="F3">
-        <v>186.4</v>
+        <v>175.8</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -939,16 +1569,16 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>4.2</v>
+        <v>9.4</v>
       </c>
       <c r="D4">
-        <v>19.7</v>
+        <v>20.7</v>
       </c>
       <c r="E4">
-        <v>49.4</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="F4">
-        <v>185.2</v>
+        <v>203.1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -956,16 +1586,16 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>6.6</v>
+        <v>9.6</v>
       </c>
       <c r="D5">
-        <v>20.9</v>
+        <v>17.2</v>
       </c>
       <c r="E5">
-        <v>50.5</v>
+        <v>44.6</v>
       </c>
       <c r="F5">
-        <v>189.4</v>
+        <v>193.4</v>
       </c>
     </row>
   </sheetData>
@@ -978,7 +1608,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F5" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,16 +1643,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>3.3</v>
+        <v>14.5</v>
       </c>
       <c r="D3">
-        <v>15.5</v>
+        <v>20.5</v>
       </c>
       <c r="E3">
-        <v>48.2</v>
+        <v>44.4</v>
       </c>
       <c r="F3">
-        <v>187.8</v>
+        <v>186.4</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1030,16 +1660,16 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>4.4000000000000004</v>
+        <v>4.2</v>
       </c>
       <c r="D4">
-        <v>11.2</v>
+        <v>19.7</v>
       </c>
       <c r="E4">
-        <v>44.8</v>
+        <v>49.4</v>
       </c>
       <c r="F4">
-        <v>193</v>
+        <v>185.2</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1047,16 +1677,16 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>12.9</v>
+        <v>6.6</v>
       </c>
       <c r="D5">
-        <v>23.4</v>
+        <v>20.9</v>
       </c>
       <c r="E5">
-        <v>67</v>
+        <v>50.5</v>
       </c>
       <c r="F5">
-        <v>192.2</v>
+        <v>189.4</v>
       </c>
     </row>
   </sheetData>
@@ -1069,7 +1699,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F5" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,16 +1734,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>5.5</v>
+        <v>3.3</v>
       </c>
       <c r="D3">
-        <v>16.2</v>
+        <v>15.5</v>
       </c>
       <c r="E3">
-        <v>43.6</v>
+        <v>48.2</v>
       </c>
       <c r="F3">
-        <v>185.5</v>
+        <v>187.8</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1121,16 +1751,16 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>9.1</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D4">
-        <v>16.2</v>
+        <v>11.2</v>
       </c>
       <c r="E4">
-        <v>43.3</v>
+        <v>44.8</v>
       </c>
       <c r="F4">
-        <v>185.5</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1138,16 +1768,16 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>9.9</v>
+        <v>12.9</v>
       </c>
       <c r="D5">
-        <v>16.5</v>
+        <v>23.4</v>
       </c>
       <c r="E5">
-        <v>44.1</v>
+        <v>67</v>
       </c>
       <c r="F5">
-        <v>187.3</v>
+        <v>192.2</v>
       </c>
     </row>
   </sheetData>
@@ -1160,7 +1790,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F5" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,16 +1825,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>7.6</v>
+        <v>5.5</v>
       </c>
       <c r="D3">
-        <v>25.9</v>
+        <v>16.2</v>
       </c>
       <c r="E3">
-        <v>41.7</v>
+        <v>43.6</v>
       </c>
       <c r="F3">
-        <v>190.8</v>
+        <v>185.5</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1212,16 +1842,16 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>9.6</v>
+        <v>9.1</v>
       </c>
       <c r="D4">
-        <v>20.399999999999999</v>
+        <v>16.2</v>
       </c>
       <c r="E4">
-        <v>48.4</v>
+        <v>43.3</v>
       </c>
       <c r="F4">
-        <v>199.4</v>
+        <v>185.5</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1229,16 +1859,16 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>9.9</v>
       </c>
       <c r="D5">
-        <v>20.3</v>
+        <v>16.5</v>
       </c>
       <c r="E5">
-        <v>48.7</v>
+        <v>44.1</v>
       </c>
       <c r="F5">
-        <v>202.2</v>
+        <v>187.3</v>
       </c>
     </row>
   </sheetData>
@@ -1251,7 +1881,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="F5" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,16 +1916,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>10.9</v>
+        <v>7.6</v>
       </c>
       <c r="D3">
-        <v>15.9</v>
+        <v>25.9</v>
       </c>
       <c r="E3">
-        <v>40.299999999999997</v>
+        <v>41.7</v>
       </c>
       <c r="F3">
-        <v>187</v>
+        <v>190.8</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1303,16 +1933,16 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>10.199999999999999</v>
+        <v>9.6</v>
       </c>
       <c r="D4">
         <v>20.399999999999999</v>
       </c>
       <c r="E4">
-        <v>47.1</v>
+        <v>48.4</v>
       </c>
       <c r="F4">
-        <v>182.6</v>
+        <v>199.4</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1320,16 +1950,16 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>11.1</v>
+        <v>10</v>
       </c>
       <c r="D5">
-        <v>19.2</v>
+        <v>20.3</v>
       </c>
       <c r="E5">
-        <v>47.1</v>
+        <v>48.7</v>
       </c>
       <c r="F5">
-        <v>186</v>
+        <v>202.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added expert user data
</commit_message>
<xml_diff>
--- a/data/userdata-micropipette-10-16-15.xlsx
+++ b/data/userdata-micropipette-10-16-15.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22455" windowHeight="8610" firstSheet="1" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22455" windowHeight="8610"/>
   </bookViews>
   <sheets>
     <sheet name="All Data" sheetId="14" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="10">
   <si>
     <t>Trial</t>
   </si>
@@ -388,18 +388,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -415,13 +416,31 @@
       <c r="F1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>20</v>
+      </c>
+      <c r="M1">
+        <v>50</v>
+      </c>
+      <c r="N1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -437,8 +456,23 @@
       <c r="F3">
         <v>184</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>10.3</v>
+      </c>
+      <c r="L3">
+        <v>20.3</v>
+      </c>
+      <c r="M3">
+        <v>49.3</v>
+      </c>
+      <c r="N3">
+        <v>192.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -454,8 +488,23 @@
       <c r="F4">
         <v>185.7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>10.3</v>
+      </c>
+      <c r="L4">
+        <v>20.6</v>
+      </c>
+      <c r="M4">
+        <v>49.1</v>
+      </c>
+      <c r="N4">
+        <v>192.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -471,8 +520,23 @@
       <c r="F5">
         <v>186.4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>9.1</v>
+      </c>
+      <c r="L5">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="M5">
+        <v>48.7</v>
+      </c>
+      <c r="N5">
+        <v>191.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -488,8 +552,23 @@
       <c r="F6">
         <v>176.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>10</v>
+      </c>
+      <c r="L6">
+        <v>20</v>
+      </c>
+      <c r="M6">
+        <v>50</v>
+      </c>
+      <c r="N6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -505,8 +584,11 @@
       <c r="F7">
         <v>182.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -522,8 +604,23 @@
       <c r="F8">
         <v>193.7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L8">
+        <v>19.8</v>
+      </c>
+      <c r="M8">
+        <v>49.7</v>
+      </c>
+      <c r="N8">
+        <v>194.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -539,8 +636,23 @@
       <c r="F9">
         <v>183.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="L9">
+        <v>20.5</v>
+      </c>
+      <c r="M9">
+        <v>49.1</v>
+      </c>
+      <c r="N9">
+        <v>198.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -556,8 +668,23 @@
       <c r="F10">
         <v>183.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="K10">
+        <v>10</v>
+      </c>
+      <c r="L10">
+        <v>20.3</v>
+      </c>
+      <c r="M10">
+        <v>50.6</v>
+      </c>
+      <c r="N10">
+        <v>200.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -574,7 +701,7 @@
         <v>187.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -591,7 +718,7 @@
         <v>175.8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -608,7 +735,7 @@
         <v>203.1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -625,7 +752,7 @@
         <v>193.4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -642,7 +769,7 @@
         <v>186.4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1172,8 +1299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,15 +1334,51 @@
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="C3">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D3">
+        <v>19.8</v>
+      </c>
+      <c r="E3">
+        <v>49.7</v>
+      </c>
+      <c r="F3">
+        <v>194.1</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
+      <c r="C4">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="D4">
+        <v>20.5</v>
+      </c>
+      <c r="E4">
+        <v>49.1</v>
+      </c>
+      <c r="F4">
+        <v>198.8</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>20.3</v>
+      </c>
+      <c r="E5">
+        <v>50.6</v>
+      </c>
+      <c r="F5">
+        <v>200.4</v>
       </c>
     </row>
   </sheetData>
@@ -1225,12 +1388,91 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="A1:F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>10</v>
+      </c>
+      <c r="D1">
+        <v>20</v>
+      </c>
+      <c r="E1">
+        <v>50</v>
+      </c>
+      <c r="F1">
+        <v>200</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>10.3</v>
+      </c>
+      <c r="D3">
+        <v>20.3</v>
+      </c>
+      <c r="E3">
+        <v>49.3</v>
+      </c>
+      <c r="F3">
+        <v>192.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>10.3</v>
+      </c>
+      <c r="D4">
+        <v>20.6</v>
+      </c>
+      <c r="E4">
+        <v>49.1</v>
+      </c>
+      <c r="F4">
+        <v>192.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>9.1</v>
+      </c>
+      <c r="D5">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="E5">
+        <v>48.7</v>
+      </c>
+      <c r="F5">
+        <v>191.4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
added analysis of expert data
</commit_message>
<xml_diff>
--- a/data/userdata-micropipette-10-16-15.xlsx
+++ b/data/userdata-micropipette-10-16-15.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="10">
   <si>
     <t>Trial</t>
   </si>
@@ -391,7 +391,7 @@
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,20 +552,20 @@
       <c r="F6">
         <v>176.5</v>
       </c>
-      <c r="J6" t="s">
+      <c r="I6">
         <v>1</v>
       </c>
       <c r="K6">
-        <v>10</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="L6">
-        <v>20</v>
+        <v>19.8</v>
       </c>
       <c r="M6">
-        <v>50</v>
+        <v>49.7</v>
       </c>
       <c r="N6">
-        <v>200</v>
+        <v>194.1</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -584,8 +584,20 @@
       <c r="F7">
         <v>182.6</v>
       </c>
-      <c r="I7" t="s">
-        <v>0</v>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="L7">
+        <v>20.5</v>
+      </c>
+      <c r="M7">
+        <v>49.1</v>
+      </c>
+      <c r="N7">
+        <v>198.8</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -605,19 +617,19 @@
         <v>193.7</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K8">
-        <v>9.1999999999999993</v>
+        <v>10</v>
       </c>
       <c r="L8">
-        <v>19.8</v>
+        <v>20.3</v>
       </c>
       <c r="M8">
-        <v>49.7</v>
+        <v>50.6</v>
       </c>
       <c r="N8">
-        <v>194.1</v>
+        <v>200.4</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -636,21 +648,6 @@
       <c r="F9">
         <v>183.9</v>
       </c>
-      <c r="I9">
-        <v>2</v>
-      </c>
-      <c r="K9">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="L9">
-        <v>20.5</v>
-      </c>
-      <c r="M9">
-        <v>49.1</v>
-      </c>
-      <c r="N9">
-        <v>198.8</v>
-      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -668,20 +665,24 @@
       <c r="F10">
         <v>183.1</v>
       </c>
-      <c r="I10">
-        <v>3</v>
-      </c>
-      <c r="K10">
-        <v>10</v>
-      </c>
-      <c r="L10">
-        <v>20.3</v>
-      </c>
-      <c r="M10">
-        <v>50.6</v>
-      </c>
-      <c r="N10">
-        <v>200.4</v>
+      <c r="I10" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="2">
+        <f>AVERAGE(K3:K8)</f>
+        <v>9.7833333333333332</v>
+      </c>
+      <c r="L10" s="2">
+        <f>AVERAGE(L3:L8)</f>
+        <v>20.066666666666666</v>
+      </c>
+      <c r="M10" s="2">
+        <f>AVERAGE(M3:M8)</f>
+        <v>49.416666666666664</v>
+      </c>
+      <c r="N10" s="2">
+        <f>AVERAGE(N3:N8)</f>
+        <v>194.9666666666667</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -717,6 +718,25 @@
       <c r="F12">
         <v>175.8</v>
       </c>
+      <c r="I12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12" s="1">
+        <f>((K10-10)/10)</f>
+        <v>-2.1666666666666678E-2</v>
+      </c>
+      <c r="L12" s="1">
+        <f>(L10-20)/20</f>
+        <v>3.3333333333333214E-3</v>
+      </c>
+      <c r="M12" s="1">
+        <f>(M10-50)/50</f>
+        <v>-1.1666666666666714E-2</v>
+      </c>
+      <c r="N12" s="1">
+        <f>(N10-200)/200</f>
+        <v>-2.5166666666666514E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -733,6 +753,25 @@
       </c>
       <c r="F13">
         <v>203.1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" s="2">
+        <f>(K5-K10)</f>
+        <v>-0.68333333333333357</v>
+      </c>
+      <c r="L13" s="2">
+        <f>(L5-L10)</f>
+        <v>-1.1666666666666679</v>
+      </c>
+      <c r="M13" s="2">
+        <f>(M8-M10)</f>
+        <v>1.1833333333333371</v>
+      </c>
+      <c r="N13" s="2">
+        <f>(N8-N10)</f>
+        <v>5.4333333333333087</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added expert data plots
</commit_message>
<xml_diff>
--- a/data/userdata-micropipette-10-16-15.xlsx
+++ b/data/userdata-micropipette-10-16-15.xlsx
@@ -352,11 +352,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="433090688"/>
-        <c:axId val="433093408"/>
+        <c:axId val="-974317920"/>
+        <c:axId val="-974324448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="433090688"/>
+        <c:axId val="-974317920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -412,12 +412,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="433093408"/>
+        <c:crossAx val="-974324448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="433093408"/>
+        <c:axId val="-974324448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="100"/>
@@ -470,7 +470,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="433090688"/>
+        <c:crossAx val="-974317920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -729,11 +729,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="433094496"/>
-        <c:axId val="433085248"/>
+        <c:axId val="-974309760"/>
+        <c:axId val="-974313024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="433094496"/>
+        <c:axId val="-974309760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -789,12 +789,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="433085248"/>
+        <c:crossAx val="-974313024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="433085248"/>
+        <c:axId val="-974313024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -851,7 +851,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="433094496"/>
+        <c:crossAx val="-974309760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1110,11 +1110,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="246173248"/>
-        <c:axId val="246164000"/>
+        <c:axId val="-974315744"/>
+        <c:axId val="-974321728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="246173248"/>
+        <c:axId val="-974315744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1170,12 +1170,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246164000"/>
+        <c:crossAx val="-974321728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="246164000"/>
+        <c:axId val="-974321728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1232,7 +1232,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246173248"/>
+        <c:crossAx val="-974315744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1491,11 +1491,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="433096128"/>
-        <c:axId val="433086880"/>
+        <c:axId val="-974311936"/>
+        <c:axId val="-974320096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="433096128"/>
+        <c:axId val="-974311936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1551,12 +1551,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="433086880"/>
+        <c:crossAx val="-974320096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="433086880"/>
+        <c:axId val="-974320096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1613,7 +1613,1265 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="433096128"/>
+        <c:crossAx val="-974311936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>200µL</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'All Data'!$N$3:$N$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>192.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>192.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>191.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>194.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>198.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-884286416"/>
+        <c:axId val="-884286960"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-884286416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-884286960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-884286960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="150"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-884286416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>50µL</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'All Data'!$M$3:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>49.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>49.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-974318464"/>
+        <c:axId val="-884285328"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-974318464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-884285328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-884285328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-974318464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>20µL</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'All Data'!$L$3:$L$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>20.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-652419952"/>
+        <c:axId val="-652407440"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-652419952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-652407440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-652407440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-652419952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>10µL</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'All Data'!$K$3:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-652422672"/>
+        <c:axId val="-652412336"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-652422672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-652412336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-652412336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-652422672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1822,6 +3080,166 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3371,6 +4789,2070 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3891,15 +7373,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>328612</xdr:colOff>
+      <xdr:colOff>271462</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>461962</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>404812</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4003,6 +7485,126 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>538162</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>233362</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>517921</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>158352</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>232171</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>44052</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>29765</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>98821</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>351233</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>175021</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>17859</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>3571</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>339327</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>79771</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4276,8 +7878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q78" sqref="Q78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added 50x reliability data
</commit_message>
<xml_diff>
--- a/data/userdata-micropipette-10-16-15.xlsx
+++ b/data/userdata-micropipette-10-16-15.xlsx
@@ -9,22 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22455" windowHeight="8610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22455" windowHeight="8610" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="All Data" sheetId="14" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId7"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId8"/>
-    <sheet name="Sheet8" sheetId="8" r:id="rId9"/>
-    <sheet name="Sheet9" sheetId="9" r:id="rId10"/>
-    <sheet name="Sheet10" sheetId="12" r:id="rId11"/>
-    <sheet name="Expert 1" sheetId="10" r:id="rId12"/>
-    <sheet name="Expert 2" sheetId="13" r:id="rId13"/>
+    <sheet name="50x 100uL" sheetId="15" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId6"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId7"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId8"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId9"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId10"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId11"/>
+    <sheet name="Sheet10" sheetId="12" r:id="rId12"/>
+    <sheet name="Expert 1" sheetId="10" r:id="rId13"/>
+    <sheet name="Expert 2" sheetId="13" r:id="rId14"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="11">
   <si>
     <t>Trial</t>
   </si>
@@ -66,6 +67,9 @@
   </si>
   <si>
     <t>200µL</t>
+  </si>
+  <si>
+    <t>100uL</t>
   </si>
 </sst>
 </file>
@@ -352,11 +356,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-974317920"/>
-        <c:axId val="-974324448"/>
+        <c:axId val="-1592966256"/>
+        <c:axId val="-1592971696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-974317920"/>
+        <c:axId val="-1592966256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -412,12 +416,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-974324448"/>
+        <c:crossAx val="-1592971696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-974324448"/>
+        <c:axId val="-1592971696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="100"/>
@@ -470,7 +474,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-974317920"/>
+        <c:crossAx val="-1592966256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -729,11 +733,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-974309760"/>
-        <c:axId val="-974313024"/>
+        <c:axId val="-1594245712"/>
+        <c:axId val="-1594238640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-974309760"/>
+        <c:axId val="-1594245712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -789,12 +793,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-974313024"/>
+        <c:crossAx val="-1594238640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-974313024"/>
+        <c:axId val="-1594238640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -851,7 +855,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-974309760"/>
+        <c:crossAx val="-1594245712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -940,7 +944,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1110,11 +1113,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-974315744"/>
-        <c:axId val="-974321728"/>
+        <c:axId val="-1465192976"/>
+        <c:axId val="-1465190800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-974315744"/>
+        <c:axId val="-1465192976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1170,12 +1173,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-974321728"/>
+        <c:crossAx val="-1465190800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-974321728"/>
+        <c:axId val="-1465190800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1232,7 +1235,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-974315744"/>
+        <c:crossAx val="-1465192976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1321,7 +1324,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1491,11 +1493,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-974311936"/>
-        <c:axId val="-974320096"/>
+        <c:axId val="-1465179376"/>
+        <c:axId val="-1465191888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-974311936"/>
+        <c:axId val="-1465179376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1551,12 +1553,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-974320096"/>
+        <c:crossAx val="-1465191888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-974320096"/>
+        <c:axId val="-1465191888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1613,7 +1615,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-974311936"/>
+        <c:crossAx val="-1465179376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1809,11 +1811,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-884286416"/>
-        <c:axId val="-884286960"/>
+        <c:axId val="-1465186992"/>
+        <c:axId val="-1465190256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-884286416"/>
+        <c:axId val="-1465186992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1869,12 +1871,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-884286960"/>
+        <c:crossAx val="-1465190256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-884286960"/>
+        <c:axId val="-1465190256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="150"/>
@@ -1932,7 +1934,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-884286416"/>
+        <c:crossAx val="-1465186992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2122,11 +2124,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-974318464"/>
-        <c:axId val="-884285328"/>
+        <c:axId val="-1465189168"/>
+        <c:axId val="-1465186448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-974318464"/>
+        <c:axId val="-1465189168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2182,12 +2184,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-884285328"/>
+        <c:crossAx val="-1465186448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-884285328"/>
+        <c:axId val="-1465186448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2245,7 +2247,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-974318464"/>
+        <c:crossAx val="-1465189168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2337,7 +2339,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2435,11 +2436,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-652419952"/>
-        <c:axId val="-652407440"/>
+        <c:axId val="-1465188080"/>
+        <c:axId val="-1465178288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-652419952"/>
+        <c:axId val="-1465188080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2495,12 +2496,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-652407440"/>
+        <c:crossAx val="-1465178288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-652407440"/>
+        <c:axId val="-1465178288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2558,7 +2559,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-652419952"/>
+        <c:crossAx val="-1465188080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2650,7 +2651,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2748,11 +2748,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-652422672"/>
-        <c:axId val="-652412336"/>
+        <c:axId val="-1465184272"/>
+        <c:axId val="-1465183728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-652422672"/>
+        <c:axId val="-1465184272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2808,12 +2808,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-652412336"/>
+        <c:crossAx val="-1465183728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-652412336"/>
+        <c:axId val="-1465183728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2871,7 +2871,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-652422672"/>
+        <c:crossAx val="-1465184272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7878,7 +7878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="Q78" sqref="Q78"/>
     </sheetView>
   </sheetViews>
@@ -8684,16 +8684,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>10.9</v>
+        <v>7.6</v>
       </c>
       <c r="D3">
-        <v>15.9</v>
+        <v>25.9</v>
       </c>
       <c r="E3">
-        <v>40.299999999999997</v>
+        <v>41.7</v>
       </c>
       <c r="F3">
-        <v>187</v>
+        <v>190.8</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -8701,16 +8701,16 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>10.199999999999999</v>
+        <v>9.6</v>
       </c>
       <c r="D4">
         <v>20.399999999999999</v>
       </c>
       <c r="E4">
-        <v>47.1</v>
+        <v>48.4</v>
       </c>
       <c r="F4">
-        <v>182.6</v>
+        <v>199.4</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -8718,16 +8718,16 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>11.1</v>
+        <v>10</v>
       </c>
       <c r="D5">
-        <v>19.2</v>
+        <v>20.3</v>
       </c>
       <c r="E5">
-        <v>47.1</v>
+        <v>48.7</v>
       </c>
       <c r="F5">
-        <v>186</v>
+        <v>202.2</v>
       </c>
     </row>
   </sheetData>
@@ -8736,6 +8736,97 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="A3:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>10</v>
+      </c>
+      <c r="D1">
+        <v>20</v>
+      </c>
+      <c r="E1">
+        <v>50</v>
+      </c>
+      <c r="F1">
+        <v>200</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>10.9</v>
+      </c>
+      <c r="D3">
+        <v>15.9</v>
+      </c>
+      <c r="E3">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="F3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D4">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="E4">
+        <v>47.1</v>
+      </c>
+      <c r="F4">
+        <v>182.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>11.1</v>
+      </c>
+      <c r="D5">
+        <v>19.2</v>
+      </c>
+      <c r="E5">
+        <v>47.1</v>
+      </c>
+      <c r="F5">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -8823,7 +8914,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -8914,7 +9005,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -9006,6 +9097,478 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>97.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A51" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>98.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>97.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>96.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>96.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>97.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>97.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>96.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>96.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>99.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>95.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>95.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>100.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>97.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>99.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>95.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>96.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>95.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>96.3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>97.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>98.9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>97.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>96.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>96.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>95.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>95.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>95.1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>95.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f>A36+1</f>
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>96.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>95.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>96.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>95.1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>95.7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>95.9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>95.4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>95.2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>96.2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>99.1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>97.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>97.1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>98.6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>98.4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>94.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -9093,97 +9656,6 @@
       </c>
       <c r="F5">
         <v>186.4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="A3:F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>10</v>
-      </c>
-      <c r="D1">
-        <v>20</v>
-      </c>
-      <c r="E1">
-        <v>50</v>
-      </c>
-      <c r="F1">
-        <v>200</v>
-      </c>
-      <c r="J1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>3.8</v>
-      </c>
-      <c r="D3">
-        <v>22.4</v>
-      </c>
-      <c r="E3">
-        <v>48.3</v>
-      </c>
-      <c r="F3">
-        <v>176.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>7.4</v>
-      </c>
-      <c r="D4">
-        <v>16.2</v>
-      </c>
-      <c r="E4">
-        <v>49</v>
-      </c>
-      <c r="F4">
-        <v>182.6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="D5">
-        <v>22.3</v>
-      </c>
-      <c r="E5">
-        <v>48.8</v>
-      </c>
-      <c r="F5">
-        <v>193.7</v>
       </c>
     </row>
   </sheetData>
@@ -9231,16 +9703,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>6.4</v>
+        <v>3.8</v>
       </c>
       <c r="D3">
-        <v>17.8</v>
+        <v>22.4</v>
       </c>
       <c r="E3">
-        <v>38.799999999999997</v>
+        <v>48.3</v>
       </c>
       <c r="F3">
-        <v>183.9</v>
+        <v>176.5</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -9248,16 +9720,16 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>6.5</v>
+        <v>7.4</v>
       </c>
       <c r="D4">
-        <v>16.3</v>
+        <v>16.2</v>
       </c>
       <c r="E4">
-        <v>38.299999999999997</v>
+        <v>49</v>
       </c>
       <c r="F4">
-        <v>183.1</v>
+        <v>182.6</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -9265,16 +9737,16 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>7.8</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="D5">
-        <v>13.5</v>
+        <v>22.3</v>
       </c>
       <c r="E5">
-        <v>37.799999999999997</v>
+        <v>48.8</v>
       </c>
       <c r="F5">
-        <v>187.5</v>
+        <v>193.7</v>
       </c>
     </row>
   </sheetData>
@@ -9322,16 +9794,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>7.3</v>
+        <v>6.4</v>
       </c>
       <c r="D3">
-        <v>9.8000000000000007</v>
+        <v>17.8</v>
       </c>
       <c r="E3">
-        <v>44.7</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="F3">
-        <v>175.8</v>
+        <v>183.9</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -9339,16 +9811,16 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>9.4</v>
+        <v>6.5</v>
       </c>
       <c r="D4">
-        <v>20.7</v>
+        <v>16.3</v>
       </c>
       <c r="E4">
         <v>38.299999999999997</v>
       </c>
       <c r="F4">
-        <v>203.1</v>
+        <v>183.1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -9356,16 +9828,16 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>9.6</v>
+        <v>7.8</v>
       </c>
       <c r="D5">
-        <v>17.2</v>
+        <v>13.5</v>
       </c>
       <c r="E5">
-        <v>44.6</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="F5">
-        <v>193.4</v>
+        <v>187.5</v>
       </c>
     </row>
   </sheetData>
@@ -9413,16 +9885,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>14.5</v>
+        <v>7.3</v>
       </c>
       <c r="D3">
-        <v>20.5</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="E3">
-        <v>44.4</v>
+        <v>44.7</v>
       </c>
       <c r="F3">
-        <v>186.4</v>
+        <v>175.8</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -9430,16 +9902,16 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>4.2</v>
+        <v>9.4</v>
       </c>
       <c r="D4">
-        <v>19.7</v>
+        <v>20.7</v>
       </c>
       <c r="E4">
-        <v>49.4</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="F4">
-        <v>185.2</v>
+        <v>203.1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -9447,16 +9919,16 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>6.6</v>
+        <v>9.6</v>
       </c>
       <c r="D5">
-        <v>20.9</v>
+        <v>17.2</v>
       </c>
       <c r="E5">
-        <v>50.5</v>
+        <v>44.6</v>
       </c>
       <c r="F5">
-        <v>189.4</v>
+        <v>193.4</v>
       </c>
     </row>
   </sheetData>
@@ -9504,16 +9976,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>3.3</v>
+        <v>14.5</v>
       </c>
       <c r="D3">
-        <v>15.5</v>
+        <v>20.5</v>
       </c>
       <c r="E3">
-        <v>48.2</v>
+        <v>44.4</v>
       </c>
       <c r="F3">
-        <v>187.8</v>
+        <v>186.4</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -9521,16 +9993,16 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>4.4000000000000004</v>
+        <v>4.2</v>
       </c>
       <c r="D4">
-        <v>11.2</v>
+        <v>19.7</v>
       </c>
       <c r="E4">
-        <v>44.8</v>
+        <v>49.4</v>
       </c>
       <c r="F4">
-        <v>193</v>
+        <v>185.2</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -9538,16 +10010,16 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>12.9</v>
+        <v>6.6</v>
       </c>
       <c r="D5">
-        <v>23.4</v>
+        <v>20.9</v>
       </c>
       <c r="E5">
-        <v>67</v>
+        <v>50.5</v>
       </c>
       <c r="F5">
-        <v>192.2</v>
+        <v>189.4</v>
       </c>
     </row>
   </sheetData>
@@ -9595,16 +10067,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>5.5</v>
+        <v>3.3</v>
       </c>
       <c r="D3">
-        <v>16.2</v>
+        <v>15.5</v>
       </c>
       <c r="E3">
-        <v>43.6</v>
+        <v>48.2</v>
       </c>
       <c r="F3">
-        <v>185.5</v>
+        <v>187.8</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -9612,16 +10084,16 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>9.1</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D4">
-        <v>16.2</v>
+        <v>11.2</v>
       </c>
       <c r="E4">
-        <v>43.3</v>
+        <v>44.8</v>
       </c>
       <c r="F4">
-        <v>185.5</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -9629,16 +10101,16 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>9.9</v>
+        <v>12.9</v>
       </c>
       <c r="D5">
-        <v>16.5</v>
+        <v>23.4</v>
       </c>
       <c r="E5">
-        <v>44.1</v>
+        <v>67</v>
       </c>
       <c r="F5">
-        <v>187.3</v>
+        <v>192.2</v>
       </c>
     </row>
   </sheetData>
@@ -9686,16 +10158,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>7.6</v>
+        <v>5.5</v>
       </c>
       <c r="D3">
-        <v>25.9</v>
+        <v>16.2</v>
       </c>
       <c r="E3">
-        <v>41.7</v>
+        <v>43.6</v>
       </c>
       <c r="F3">
-        <v>190.8</v>
+        <v>185.5</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -9703,16 +10175,16 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>9.6</v>
+        <v>9.1</v>
       </c>
       <c r="D4">
-        <v>20.399999999999999</v>
+        <v>16.2</v>
       </c>
       <c r="E4">
-        <v>48.4</v>
+        <v>43.3</v>
       </c>
       <c r="F4">
-        <v>199.4</v>
+        <v>185.5</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -9720,16 +10192,16 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>9.9</v>
       </c>
       <c r="D5">
-        <v>20.3</v>
+        <v>16.5</v>
       </c>
       <c r="E5">
-        <v>48.7</v>
+        <v>44.1</v>
       </c>
       <c r="F5">
-        <v>202.2</v>
+        <v>187.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added average and SD
</commit_message>
<xml_diff>
--- a/data/userdata-micropipette-10-16-15.xlsx
+++ b/data/userdata-micropipette-10-16-15.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="13">
   <si>
     <t>Trial</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>100uL</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Standard Deviation S or P</t>
   </si>
 </sst>
 </file>
@@ -356,11 +362,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1592966256"/>
-        <c:axId val="-1592971696"/>
+        <c:axId val="1868354256"/>
+        <c:axId val="1868352080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1592966256"/>
+        <c:axId val="1868354256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -416,12 +422,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1592971696"/>
+        <c:crossAx val="1868352080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1592971696"/>
+        <c:axId val="1868352080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="100"/>
@@ -474,7 +480,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1592966256"/>
+        <c:crossAx val="1868354256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -563,7 +569,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -733,11 +738,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1594245712"/>
-        <c:axId val="-1594238640"/>
+        <c:axId val="1868360240"/>
+        <c:axId val="1868349904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1594245712"/>
+        <c:axId val="1868360240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -793,12 +798,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1594238640"/>
+        <c:crossAx val="1868349904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1594238640"/>
+        <c:axId val="1868349904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -855,7 +860,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1594245712"/>
+        <c:crossAx val="1868360240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1113,11 +1118,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1465192976"/>
-        <c:axId val="-1465190800"/>
+        <c:axId val="1868349360"/>
+        <c:axId val="1868356976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1465192976"/>
+        <c:axId val="1868349360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1173,12 +1178,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1465190800"/>
+        <c:crossAx val="1868356976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1465190800"/>
+        <c:axId val="1868356976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1235,7 +1240,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1465192976"/>
+        <c:crossAx val="1868349360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1493,11 +1498,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1465179376"/>
-        <c:axId val="-1465191888"/>
+        <c:axId val="1868347184"/>
+        <c:axId val="1868347728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1465179376"/>
+        <c:axId val="1868347184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1553,12 +1558,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1465191888"/>
+        <c:crossAx val="1868347728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1465191888"/>
+        <c:axId val="1868347728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1615,7 +1620,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1465179376"/>
+        <c:crossAx val="1868347184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1713,7 +1718,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1811,11 +1815,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1465186992"/>
-        <c:axId val="-1465190256"/>
+        <c:axId val="1868346640"/>
+        <c:axId val="1868357520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1465186992"/>
+        <c:axId val="1868346640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1871,12 +1875,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1465190256"/>
+        <c:crossAx val="1868357520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1465190256"/>
+        <c:axId val="1868357520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="150"/>
@@ -1934,7 +1938,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1465186992"/>
+        <c:crossAx val="1868346640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2026,7 +2030,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2124,11 +2127,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1465189168"/>
-        <c:axId val="-1465186448"/>
+        <c:axId val="1868352624"/>
+        <c:axId val="1868353168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1465189168"/>
+        <c:axId val="1868352624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2184,12 +2187,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1465186448"/>
+        <c:crossAx val="1868353168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1465186448"/>
+        <c:axId val="1868353168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2247,7 +2250,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1465189168"/>
+        <c:crossAx val="1868352624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2436,11 +2439,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1465188080"/>
-        <c:axId val="-1465178288"/>
+        <c:axId val="1916165808"/>
+        <c:axId val="1916162544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1465188080"/>
+        <c:axId val="1916165808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2496,12 +2499,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1465178288"/>
+        <c:crossAx val="1916162544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1465178288"/>
+        <c:axId val="1916162544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2559,7 +2562,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1465188080"/>
+        <c:crossAx val="1916165808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2748,11 +2751,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1465184272"/>
-        <c:axId val="-1465183728"/>
+        <c:axId val="1916175056"/>
+        <c:axId val="1916174512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1465184272"/>
+        <c:axId val="1916175056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2808,12 +2811,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1465183728"/>
+        <c:crossAx val="1916174512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1465183728"/>
+        <c:axId val="1916174512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2871,7 +2874,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1465184272"/>
+        <c:crossAx val="1916175056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9098,13 +9101,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -9536,7 +9542,7 @@
         <v>97.1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -9545,7 +9551,7 @@
         <v>98.6</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -9554,13 +9560,35 @@
         <v>98.4</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="B51">
         <v>94.1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>11</v>
+      </c>
+      <c r="B53">
+        <f>AVERAGE(B2:B51)</f>
+        <v>96.768000000000015</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54">
+        <f>_xlfn.STDEV.P(B2:B51)</f>
+        <v>1.3606527845119052</v>
+      </c>
+      <c r="C54">
+        <f>_xlfn.STDEV.S(B2:B51)</f>
+        <v>1.3744668725267519</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added SD of sample
</commit_message>
<xml_diff>
--- a/data/userdata-micropipette-10-16-15.xlsx
+++ b/data/userdata-micropipette-10-16-15.xlsx
@@ -75,7 +75,7 @@
     <t>Average</t>
   </si>
   <si>
-    <t>Standard Deviation S or P</t>
+    <t>Standard Deviation S</t>
   </si>
 </sst>
 </file>
@@ -362,11 +362,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1868354256"/>
-        <c:axId val="1868352080"/>
+        <c:axId val="-1517026032"/>
+        <c:axId val="-1517013520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1868354256"/>
+        <c:axId val="-1517026032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -422,12 +422,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1868352080"/>
+        <c:crossAx val="-1517013520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1868352080"/>
+        <c:axId val="-1517013520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="100"/>
@@ -480,7 +480,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1868354256"/>
+        <c:crossAx val="-1517026032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -738,11 +738,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1868360240"/>
-        <c:axId val="1868349904"/>
+        <c:axId val="-1517027120"/>
+        <c:axId val="-1517022768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1868360240"/>
+        <c:axId val="-1517027120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -798,12 +798,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1868349904"/>
+        <c:crossAx val="-1517022768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1868349904"/>
+        <c:axId val="-1517022768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -860,7 +860,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1868360240"/>
+        <c:crossAx val="-1517027120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1118,11 +1118,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1868349360"/>
-        <c:axId val="1868356976"/>
+        <c:axId val="-1517025488"/>
+        <c:axId val="-1517018960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1868349360"/>
+        <c:axId val="-1517025488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1178,12 +1178,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1868356976"/>
+        <c:crossAx val="-1517018960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1868356976"/>
+        <c:axId val="-1517018960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1240,7 +1240,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1868349360"/>
+        <c:crossAx val="-1517025488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1498,11 +1498,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1868347184"/>
-        <c:axId val="1868347728"/>
+        <c:axId val="-1517024944"/>
+        <c:axId val="-1517017872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1868347184"/>
+        <c:axId val="-1517024944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1558,12 +1558,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1868347728"/>
+        <c:crossAx val="-1517017872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1868347728"/>
+        <c:axId val="-1517017872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1620,7 +1620,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1868347184"/>
+        <c:crossAx val="-1517024944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1815,11 +1815,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1868346640"/>
-        <c:axId val="1868357520"/>
+        <c:axId val="-1517021680"/>
+        <c:axId val="-1517020592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1868346640"/>
+        <c:axId val="-1517021680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1875,12 +1875,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1868357520"/>
+        <c:crossAx val="-1517020592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1868357520"/>
+        <c:axId val="-1517020592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="150"/>
@@ -1938,7 +1938,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1868346640"/>
+        <c:crossAx val="-1517021680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2127,11 +2127,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1868352624"/>
-        <c:axId val="1868353168"/>
+        <c:axId val="-1517016784"/>
+        <c:axId val="-1517014608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1868352624"/>
+        <c:axId val="-1517016784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2187,12 +2187,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1868353168"/>
+        <c:crossAx val="-1517014608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1868353168"/>
+        <c:axId val="-1517014608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2250,7 +2250,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1868352624"/>
+        <c:crossAx val="-1517016784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2439,11 +2439,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1916165808"/>
-        <c:axId val="1916162544"/>
+        <c:axId val="-1398493296"/>
+        <c:axId val="-1398494384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1916165808"/>
+        <c:axId val="-1398493296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2499,12 +2499,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1916162544"/>
+        <c:crossAx val="-1398494384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1916162544"/>
+        <c:axId val="-1398494384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2562,7 +2562,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1916165808"/>
+        <c:crossAx val="-1398493296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2751,11 +2751,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1916175056"/>
-        <c:axId val="1916174512"/>
+        <c:axId val="-1398502544"/>
+        <c:axId val="-1398491120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1916175056"/>
+        <c:axId val="-1398502544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2811,12 +2811,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1916174512"/>
+        <c:crossAx val="-1398491120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1916174512"/>
+        <c:axId val="-1398491120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2874,7 +2874,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1916175056"/>
+        <c:crossAx val="-1398502544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9101,10 +9101,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9542,7 +9542,7 @@
         <v>97.1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -9551,7 +9551,7 @@
         <v>98.6</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -9560,7 +9560,7 @@
         <v>98.4</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -9569,7 +9569,7 @@
         <v>94.1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -9578,15 +9578,11 @@
         <v>96.768000000000015</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>12</v>
       </c>
       <c r="B54">
-        <f>_xlfn.STDEV.P(B2:B51)</f>
-        <v>1.3606527845119052</v>
-      </c>
-      <c r="C54">
         <f>_xlfn.STDEV.S(B2:B51)</f>
         <v>1.3744668725267519</v>
       </c>

</xml_diff>